<commit_message>
Code: using NAMELIST PARAMETERS for k-values&calculate apparent k-value then k1 and k2 + calculate mean OM wt% in upper 5 cm; changed diffusion coefficients ALK, DIC;
</commit_message>
<xml_diff>
--- a/OM_degradation_rates.xlsx
+++ b/OM_degradation_rates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="131" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="318" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Calc_apparent_k" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Tromp_Boudreau" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="sed-rate" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="53">
   <si>
     <t>Examples of invariant rates used in HAMOCC</t>
   </si>
@@ -121,6 +121,63 @@
   </si>
   <si>
     <t>EXAMPLE GENIE GRIDS:</t>
+  </si>
+  <si>
+    <t>DEFAULT k = 1.0e-6</t>
+  </si>
+  <si>
+    <t>4 years</t>
+  </si>
+  <si>
+    <t> dum_D </t>
+  </si>
+  <si>
+    <t> loc_new_sed_vol Middelburg </t>
+  </si>
+  <si>
+    <t> loc_new_sed_vol GENIE </t>
+  </si>
+  <si>
+    <t> k1, k2 </t>
+  </si>
+  <si>
+    <t>  9.99999999999999955E-007  9.99999999999999955E-007</t>
+  </si>
+  <si>
+    <t> boudreau1997 oxic k1, k2 </t>
+  </si>
+  <si>
+    <t>  0.19638394253086039       1.96383942530860408E-003</t>
+  </si>
+  <si>
+    <t> dum_POC1_conc_swi </t>
+  </si>
+  <si>
+    <t> dum_POC2_conc_swi </t>
+  </si>
+  <si>
+    <t> loc_mean_OM </t>
+  </si>
+  <si>
+    <t>  </t>
+  </si>
+  <si>
+    <t>  5.27435245328635449E-002  5.27435245328635480E-004</t>
+  </si>
+  <si>
+    <t>  4.48806848341056636E-002  4.48806848341056636E-004</t>
+  </si>
+  <si>
+    <t>  4.83438195143225044E-002  4.83438195143225027E-004</t>
+  </si>
+  <si>
+    <t>  4.31183093186053093E-002  4.31183093186053080E-004</t>
+  </si>
+  <si>
+    <t>  4.94627074871127198E-002  4.94627074871127181E-004</t>
+  </si>
+  <si>
+    <t>  1.88274354166577604E-002  1.88274354166577596E-004</t>
   </si>
 </sst>
 </file>
@@ -484,7 +541,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -516,7 +573,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="3"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -528,151 +585,151 @@
                   <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0098</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0096</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0094</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0092</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.009</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0088</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0086</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0084</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0082</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.008</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0078</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0076</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0074</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0072</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.007</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0068</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0066</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0064</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0062</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.006</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.0058</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.0056</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.0054</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.0052</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.005</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.0048</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.0046</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.0044</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.0042</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.004</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.0038</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.0036</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.0034</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.0032</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.003</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.0028</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.0026</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.0024</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.0022</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.002</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.0018</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.0016</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.0014</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.0012</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.001</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.0008</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.0006</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.0004</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.0002</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -860,7 +917,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="3"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1204,7 +1261,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="3"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1548,7 +1605,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="3"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1869,11 +1926,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="41094556"/>
-        <c:axId val="14801883"/>
+        <c:axId val="76981233"/>
+        <c:axId val="24182822"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="41094556"/>
+        <c:axId val="76981233"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1889,11 +1946,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="14801883"/>
+        <c:crossAx val="24182822"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="14801883"/>
+        <c:axId val="24182822"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1918,7 +1975,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="41094556"/>
+        <c:crossAx val="76981233"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1958,15 +2015,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>781560</xdr:colOff>
+      <xdr:colOff>808560</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>90000</xdr:rowOff>
+      <xdr:rowOff>81000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>335520</xdr:colOff>
+      <xdr:colOff>362160</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>82440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1974,8 +2031,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7210080" y="252360"/>
-        <a:ext cx="8536680" cy="6772320"/>
+        <a:off x="7237080" y="243360"/>
+        <a:ext cx="8536320" cy="6771960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1995,8 +2052,8 @@
   </sheetPr>
   <dimension ref="C1:O61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1:O61"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4171,7 +4228,7 @@
   <dimension ref="A2:V60"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S17" activeCellId="1" sqref="C1:O61 S17"/>
+      <selection pane="topLeft" activeCell="S17" activeCellId="0" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5557,17 +5614,827 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1:O61 A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.7448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5714285714286"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>3224.39</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>3224.39</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="25" t="n">
+        <v>0.0174073913465891</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="25" t="n">
+        <v>0.0174073913465891</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="25" t="n">
+        <v>0.00905420943797329</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="25" t="n">
+        <v>0.00838855821647622</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.733567390573683</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>6.16628412805505</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="25" t="n">
+        <v>0.0105579786502628</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>6.89970872110144</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>1.85502754530844</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>1.7860288485136</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>1885.33</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="25" t="n">
+        <v>0.0665863915555153</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>1885.33</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="25" t="n">
+        <v>0.0121820294071994</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="25" t="n">
+        <v>0.0665863915555153</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="25" t="n">
+        <v>0.0112686798808896</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>4.82102591004869</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>4.7100584682048</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>9.53102565960586</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>0.126974631540773</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>3.09742234137423</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>1707.04</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>3.18462410915096</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="25" t="n">
+        <v>0.0796091569963983</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="25" t="n">
+        <v>0.0133703247435226</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>1707.04</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="25" t="n">
+        <v>0.0796091569963983</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>7.15329229537103</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="25" t="n">
+        <v>0.0124963864811004</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>4.12322934641132</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>11.2764625888247</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>0.230555884990333</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1631.73</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>2.94768993553845</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="25" t="n">
+        <v>0.0858483420562948</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>3.12901332289223</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="25" t="n">
+        <v>0.0147866557709214</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>1631.73</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>7.22104189591477</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" s="25" t="n">
+        <v>0.0858483420562948</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>4.162280894934</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H32" s="25" t="n">
+        <v>0.0141742089005532</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>11.3832671605332</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>1276.06</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>0.243740988673165</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>0.122600161613828</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <v>3.00051480320737</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="25" t="n">
+        <v>0.0162094513521557</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <v>3.19226785638621</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>9.54813216436608</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>1276.06</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>3.49452531337901</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>0.122600161613828</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>13.042611359173</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H41" s="25" t="n">
+        <v>0.0148325327507379</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>1733.14</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="25" t="n">
+        <v>0.0775543912150806</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <v>0.346713028636503</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="25" t="n">
+        <v>0.0270356845332595</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <v>2.57417709180406</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <v>2.87224516711447</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>14.5861799249095</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>2.57887732799694</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H48" s="0" t="n">
+        <v>1733.14</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>17.1649659667583</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H49" s="25" t="n">
+        <v>0.0775543912150806</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H50" s="25" t="n">
+        <v>0.0240218462854766</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>1145.54</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>0.139727826991123</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H52" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B53" s="25" t="n">
+        <v>0.00539919856208694</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>0.787616519847601</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>1.9896617741242</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>18.7412552816673</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <v>2.61417434358327</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>3.31350624995081</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>22.0546920049182</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <v>1145.54</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G58" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <v>0.139727826991123</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G59" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H59" s="25" t="n">
+        <v>0.00467317393173504</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G60" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H60" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G61" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H61" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G62" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H62" s="0" t="n">
+        <v>0.454771937101082</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G63" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H63" s="0" t="n">
+        <v>2.23547135492507</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G64" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H64" s="0" t="n">
+        <v>2.6637119688558</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5586,7 +6453,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="20" zoomScaleNormal="20" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1:O61 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5612,7 +6479,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="20" zoomScaleNormal="20" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1:O61 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
LaTeX: added version of Sandra's comments on model description 20.06.2017
</commit_message>
<xml_diff>
--- a/OM_degradation_rates.xlsx
+++ b/OM_degradation_rates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="159" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="223" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="invariant_k" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="67">
   <si>
     <t>Experiments 13.06.2017</t>
   </si>
@@ -60,13 +60,10 @@
     <t>INCLUDED IN FIGURE</t>
   </si>
   <si>
-    <t>not ready yet</t>
-  </si>
-  <si>
     <t>parallel to 1:1</t>
   </si>
   <si>
-    <t>k1 needs  higher! </t>
+    <t>k1 needs  higher!</t>
   </si>
   <si>
     <t>k1 needs  higher!  1000M does not get further down</t>
@@ -619,7 +616,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2004,11 +2001,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="38432366"/>
-        <c:axId val="21412513"/>
+        <c:axId val="61650144"/>
+        <c:axId val="85958370"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="38432366"/>
+        <c:axId val="61650144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2024,11 +2021,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="21412513"/>
+        <c:crossAx val="85958370"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="21412513"/>
+        <c:axId val="85958370"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2053,7 +2050,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="38432366"/>
+        <c:crossAx val="61650144"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2093,15 +2090,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>73080</xdr:colOff>
+      <xdr:colOff>100080</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>54000</xdr:rowOff>
+      <xdr:rowOff>45000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>442080</xdr:colOff>
+      <xdr:colOff>468720</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>77040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2109,8 +2106,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7318080" y="216360"/>
-        <a:ext cx="8535240" cy="6770880"/>
+        <a:off x="7345080" y="207360"/>
+        <a:ext cx="8534880" cy="6770520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2130,8 +2127,8 @@
   </sheetPr>
   <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H60" activeCellId="0" sqref="H60"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B69" activeCellId="0" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2968,9 +2965,6 @@
       <c r="D66" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="E66" s="0" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="n">
@@ -2987,7 +2981,7 @@
         <v>5</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3065,7 +3059,7 @@
         <v>4</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3083,7 +3077,7 @@
         <v>5</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3131,7 +3125,7 @@
         <v>1</v>
       </c>
       <c r="H76" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3148,9 +3142,6 @@
       <c r="D77" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="E77" s="0" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="n">
@@ -3210,9 +3201,6 @@
       </c>
       <c r="D81" s="6" t="n">
         <v>10</v>
-      </c>
-      <c r="E81" s="0" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3346,7 +3334,7 @@
       <c r="C1" s="9"/>
       <c r="D1" s="3"/>
       <c r="E1" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -3361,46 +3349,46 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="O2" s="13"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>22</v>
       </c>
       <c r="F3" s="14" t="n">
         <v>0.01</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L3" s="14" t="n">
         <v>0.008</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="F4" s="16" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>27</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>5</v>
@@ -3409,13 +3397,13 @@
         <v>3</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K4" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="16" t="s">
         <v>26</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>27</v>
       </c>
       <c r="M4" s="16" t="s">
         <v>5</v>
@@ -3424,7 +3412,7 @@
         <v>3</v>
       </c>
       <c r="O4" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3890,32 +3878,32 @@
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="19"/>
       <c r="E17" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17" s="14" t="n">
         <v>0.005</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L17" s="14" t="n">
         <v>0.002</v>
       </c>
       <c r="M17" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="19"/>
       <c r="E18" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="16" t="s">
         <v>26</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>27</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>5</v>
@@ -3924,13 +3912,13 @@
         <v>3</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K18" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="16" t="s">
         <v>26</v>
-      </c>
-      <c r="L18" s="16" t="s">
-        <v>27</v>
       </c>
       <c r="M18" s="16" t="s">
         <v>5</v>
@@ -3939,7 +3927,7 @@
         <v>3</v>
       </c>
       <c r="O18" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4412,7 +4400,7 @@
       <c r="C32" s="9"/>
       <c r="D32" s="3"/>
       <c r="E32" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -4427,46 +4415,46 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="O33" s="13"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>22</v>
       </c>
       <c r="F34" s="14" t="n">
         <v>0.01</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L34" s="14" t="n">
         <v>0.008</v>
       </c>
       <c r="M34" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O34" s="13"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E35" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="16" t="s">
         <v>26</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>27</v>
       </c>
       <c r="G35" s="16" t="s">
         <v>5</v>
@@ -4475,13 +4463,13 @@
         <v>3</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K35" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L35" s="16" t="s">
         <v>26</v>
-      </c>
-      <c r="L35" s="16" t="s">
-        <v>27</v>
       </c>
       <c r="M35" s="16" t="s">
         <v>5</v>
@@ -4490,12 +4478,12 @@
         <v>3</v>
       </c>
       <c r="O35" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E36" s="17" t="n">
         <v>0.95</v>
@@ -4538,7 +4526,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E37" s="17" t="n">
         <v>0.9</v>
@@ -4581,7 +4569,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E38" s="17" t="n">
         <v>0.8</v>
@@ -4962,32 +4950,32 @@
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="19"/>
       <c r="E48" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F48" s="14" t="n">
         <v>0.005</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K48" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L48" s="14" t="n">
         <v>0.002</v>
       </c>
       <c r="M48" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O48" s="13"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="19"/>
       <c r="E49" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F49" s="16" t="s">
         <v>26</v>
-      </c>
-      <c r="F49" s="16" t="s">
-        <v>27</v>
       </c>
       <c r="G49" s="16" t="s">
         <v>5</v>
@@ -4996,13 +4984,13 @@
         <v>3</v>
       </c>
       <c r="I49" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K49" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L49" s="16" t="s">
         <v>26</v>
-      </c>
-      <c r="L49" s="16" t="s">
-        <v>27</v>
       </c>
       <c r="M49" s="16" t="s">
         <v>5</v>
@@ -5011,7 +4999,7 @@
         <v>3</v>
       </c>
       <c r="O49" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5511,32 +5499,32 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="27"/>
       <c r="E2" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" s="27"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5824,7 +5812,7 @@
         <v>2.3104E-006</v>
       </c>
       <c r="S16" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5849,7 +5837,7 @@
         <v>2.1904E-006</v>
       </c>
       <c r="S17" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5874,13 +5862,13 @@
         <v>2.0736E-006</v>
       </c>
       <c r="S18" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="T18" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="T18" s="0" t="s">
+      <c r="U18" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="U18" s="0" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6091,7 +6079,7 @@
         <v>1.3456E-006</v>
       </c>
       <c r="S25" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T25" s="0" t="n">
         <v>1195</v>
@@ -6741,7 +6729,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6901,29 +6889,29 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>3224.39</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>3224.39</v>
@@ -6931,13 +6919,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="30" t="n">
         <v>0.0174073913465891</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H4" s="30" t="n">
         <v>0.0174073913465891</v>
@@ -6945,13 +6933,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="30" t="n">
         <v>0.00905420943797329</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H5" s="30" t="n">
         <v>0.00838855821647622</v>
@@ -6959,41 +6947,41 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="G6" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.733567390573683</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>6.16628412805505</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H8" s="30" t="n">
         <v>0.0105579786502628</v>
@@ -7001,13 +6989,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>6.89970872110144</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>1.85502754530844</v>
@@ -7015,7 +7003,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G10" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>1.7860288485136</v>
@@ -7023,7 +7011,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1885.33</v>
@@ -7031,13 +7019,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="30" t="n">
         <v>0.0665863915555153</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>1885.33</v>
@@ -7045,13 +7033,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="30" t="n">
         <v>0.0121820294071994</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H13" s="30" t="n">
         <v>0.0665863915555153</v>
@@ -7059,13 +7047,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="G14" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H14" s="30" t="n">
         <v>0.0112686798808896</v>
@@ -7073,41 +7061,41 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>4.82102591004869</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>4.7100584682048</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>9.53102565960586</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>0.126974631540773</v>
@@ -7115,7 +7103,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G18" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>3.09742234137423</v>
@@ -7123,13 +7111,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1707.04</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>3.18462410915096</v>
@@ -7137,7 +7125,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="30" t="n">
         <v>0.0796091569963983</v>
@@ -7145,13 +7133,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="30" t="n">
         <v>0.0133703247435226</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>1707.04</v>
@@ -7159,13 +7147,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="G22" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H22" s="30" t="n">
         <v>0.0796091569963983</v>
@@ -7173,13 +7161,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>7.15329229537103</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H23" s="30" t="n">
         <v>0.0124963864811004</v>
@@ -7187,35 +7175,35 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>4.12322934641132</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>11.2764625888247</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G26" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>0.230555884990333</v>
@@ -7223,13 +7211,13 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>1631.73</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H27" s="0" t="n">
         <v>2.94768993553845</v>
@@ -7237,13 +7225,13 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="30" t="n">
         <v>0.0858483420562948</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>3.12901332289223</v>
@@ -7251,7 +7239,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B29" s="30" t="n">
         <v>0.0147866557709214</v>
@@ -7259,13 +7247,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="G30" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H30" s="0" t="n">
         <v>1631.73</v>
@@ -7273,13 +7261,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>7.22104189591477</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H31" s="30" t="n">
         <v>0.0858483420562948</v>
@@ -7287,13 +7275,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>4.162280894934</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H32" s="30" t="n">
         <v>0.0141742089005532</v>
@@ -7301,35 +7289,35 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>11.3832671605332</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G34" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1276.06</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H35" s="0" t="n">
         <v>0.243740988673165</v>
@@ -7337,13 +7325,13 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>0.122600161613828</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H36" s="0" t="n">
         <v>3.00051480320737</v>
@@ -7351,13 +7339,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37" s="30" t="n">
         <v>0.0162094513521557</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H37" s="0" t="n">
         <v>3.19226785638621</v>
@@ -7365,21 +7353,21 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>9.54813216436608</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H39" s="0" t="n">
         <v>1276.06</v>
@@ -7387,13 +7375,13 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>3.49452531337901</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H40" s="0" t="n">
         <v>0.122600161613828</v>
@@ -7401,13 +7389,13 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>13.042611359173</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H41" s="30" t="n">
         <v>0.0148325327507379</v>
@@ -7415,35 +7403,35 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G42" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>1733.14</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B44" s="30" t="n">
         <v>0.0775543912150806</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H44" s="0" t="n">
         <v>0.346713028636503</v>
@@ -7451,13 +7439,13 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B45" s="30" t="n">
         <v>0.0270356845332595</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H45" s="0" t="n">
         <v>2.57417709180406</v>
@@ -7465,13 +7453,13 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="G46" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H46" s="0" t="n">
         <v>2.87224516711447</v>
@@ -7479,7 +7467,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>14.5861799249095</v>
@@ -7487,13 +7475,13 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>2.57887732799694</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H48" s="0" t="n">
         <v>1733.14</v>
@@ -7501,13 +7489,13 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>17.1649659667583</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H49" s="30" t="n">
         <v>0.0775543912150806</v>
@@ -7515,7 +7503,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G50" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H50" s="30" t="n">
         <v>0.0240218462854766</v>
@@ -7523,41 +7511,41 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>1145.54</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>0.139727826991123</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53" s="30" t="n">
         <v>0.00539919856208694</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H53" s="0" t="n">
         <v>0.787616519847601</v>
@@ -7565,13 +7553,13 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="G54" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H54" s="0" t="n">
         <v>1.9896617741242</v>
@@ -7579,13 +7567,13 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>18.7412552816673</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H55" s="0" t="n">
         <v>2.61417434358327</v>
@@ -7593,7 +7581,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>3.31350624995081</v>
@@ -7601,13 +7589,13 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>22.0546920049182</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H57" s="0" t="n">
         <v>1145.54</v>
@@ -7615,7 +7603,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G58" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H58" s="0" t="n">
         <v>0.139727826991123</v>
@@ -7623,7 +7611,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G59" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H59" s="30" t="n">
         <v>0.00467317393173504</v>
@@ -7631,23 +7619,23 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G60" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G61" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G62" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H62" s="0" t="n">
         <v>0.454771937101082</v>
@@ -7655,7 +7643,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G63" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H63" s="0" t="n">
         <v>2.23547135492507</v>
@@ -7663,7 +7651,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G64" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H64" s="0" t="n">
         <v>2.6637119688558</v>

</xml_diff>

<commit_message>
more runs with Andys new hack to report global POC burial
</commit_message>
<xml_diff>
--- a/OM_degradation_rates.xlsx
+++ b/OM_degradation_rates.xlsx
@@ -81,10 +81,10 @@
     <t>config exists from 1507</t>
   </si>
   <si>
-    <t>RUNS 2808</t>
+    <t>RUNS 2808 + 2908</t>
   </si>
   <si>
-    <t>RUNS 2908</t>
+    <t>RUNS 3008</t>
   </si>
   <si>
     <t>Examples of invariant rates used in HAMOCC</t>
@@ -671,7 +671,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2056,11 +2056,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="20797966"/>
-        <c:axId val="37950487"/>
+        <c:axId val="11108035"/>
+        <c:axId val="57299512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="20797966"/>
+        <c:axId val="11108035"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2076,11 +2076,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="37950487"/>
+        <c:crossAx val="57299512"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="37950487"/>
+        <c:axId val="57299512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2105,7 +2105,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="20797966"/>
+        <c:crossAx val="11108035"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2182,8 +2182,8 @@
   </sheetPr>
   <dimension ref="A1:K156"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A131" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K139" activeCellId="0" sqref="K139"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A134" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F130" activeCellId="0" sqref="F130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>